<commit_message>
Master reduction output updates
converted 236U and 229Th signals to mV
multiplied 234tail/234 by 1000 to get to per mil
Removed upper/lower age in output
Removed significant figure values in output
</commit_message>
<xml_diff>
--- a/mad_test_2/AB12-6_AB10-bot reduction.xlsx
+++ b/mad_test_2/AB12-6_AB10-bot reduction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr showInkAnnotation="0" updateLinks="never" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/tigerb_mit_edu/Documents/Documents/MIT-WHOI stuff/other_projs/U-Th software/mad_test_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/tigerb_mit_edu/Documents/Documents/GitHub/U_Th_dating/mad_test_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CF93B1D-9213-4228-84C1-6E33F9311333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{7CF93B1D-9213-4228-84C1-6E33F9311333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{984C0FC3-491C-4091-A6E4-C66C6CB79EE6}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="U-Th data" sheetId="9" r:id="rId1"/>
@@ -3274,7 +3274,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3395,6 +3395,7 @@
     <xf numFmtId="173" fontId="13" fillId="0" borderId="0" xfId="1203" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1497">
     <cellStyle name="Bad" xfId="1267" builtinId="27"/>
@@ -4938,21 +4939,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5802,8 +5803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CA65"/>
   <sheetViews>
-    <sheetView topLeftCell="C48" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53:B62"/>
+    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6204,8 +6205,8 @@
         <f>Z4*AY4*232*E4</f>
         <v>0.31807395611086225</v>
       </c>
-      <c r="P4" s="38">
-        <f>MAX(E$4*AZ$4*AD$4*234*1000,Q4/15)</f>
+      <c r="P4" s="92">
+        <f>MAX(E$4*AZ$4*AD$4*234*1000, Q4/15)</f>
         <v>0.24690791130277173</v>
       </c>
       <c r="Q4" s="38">
@@ -12571,9 +12572,6 @@
       </c>
       <c r="M40">
         <v>54264.1420376776</v>
-      </c>
-      <c r="N40">
-        <v>398.51909564263798</v>
       </c>
       <c r="O40">
         <v>53481.246356897602</v>
@@ -42825,6 +42823,19 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
+          <x14:cfRule type="expression" priority="15" id="{069C5E89-77CD-AB4F-B109-7C367E52547F}">
+            <xm:f>AND(NOT(ISBLANK(B5)),AR5&gt;(Constants!$B$38*AQ5))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C6500"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFEB9C"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
           <x14:cfRule type="expression" priority="17" id="{EB4CD11B-4043-0640-BA98-EB4DF1B16716}">
             <xm:f>AND(NOT(ISBLANK(B5)),(AR5-AQ5)&gt;Constants!$B$37)</xm:f>
             <x14:dxf>
@@ -42834,19 +42845,6 @@
               <fill>
                 <patternFill>
                   <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="expression" priority="15" id="{069C5E89-77CD-AB4F-B109-7C367E52547F}">
-            <xm:f>AND(NOT(ISBLANK(B5)),AR5&gt;(Constants!$B$38*AQ5))</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C6500"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFEB9C"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -44285,7 +44283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4705D6-4630-4BD3-8225-74831985CAC2}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>

</xml_diff>